<commit_message>
increased font size in some figures
</commit_message>
<xml_diff>
--- a/figs/lm_results.xlsx
+++ b/figs/lm_results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Dropbox\papers\15jsalt\probtranspaper\figs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8610" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,24 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
-    <t xml:space="preserve">SW </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">HG </t>
-  </si>
-  <si>
     <t>Language</t>
   </si>
   <si>
@@ -50,12 +37,30 @@
   <si>
     <t>Bigram LM</t>
   </si>
+  <si>
+    <t>swh</t>
+  </si>
+  <si>
+    <t>nld</t>
+  </si>
+  <si>
+    <t>cmn</t>
+  </si>
+  <si>
+    <t>urd</t>
+  </si>
+  <si>
+    <t>arb</t>
+  </si>
+  <si>
+    <t>hun</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -84,6 +89,13 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,9 +126,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -131,6 +144,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -176,22 +197,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SW </c:v>
+                  <c:v>swh</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>DT </c:v>
+                  <c:v>nld</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MD </c:v>
+                  <c:v>cmn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>UR </c:v>
+                  <c:v>urd</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>AR </c:v>
+                  <c:v>arb</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>HG </c:v>
+                  <c:v>hun</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -215,7 +236,7 @@
                   <c:v>97.95</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.04</c:v>
+                  <c:v>79.040000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>92.87</c:v>
@@ -245,22 +266,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SW </c:v>
+                  <c:v>swh</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>DT </c:v>
+                  <c:v>nld</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MD </c:v>
+                  <c:v>cmn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>UR </c:v>
+                  <c:v>urd</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>AR </c:v>
+                  <c:v>arb</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>HG </c:v>
+                  <c:v>hun</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -314,22 +335,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>SW </c:v>
+                  <c:v>swh</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>DT </c:v>
+                  <c:v>nld</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>MD </c:v>
+                  <c:v>cmn</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>UR </c:v>
+                  <c:v>urd</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>AR </c:v>
+                  <c:v>arb</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>HG </c:v>
+                  <c:v>hun</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -344,7 +365,7 @@
                   <c:v>48.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.0</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>70.88</c:v>
@@ -353,7 +374,7 @@
                   <c:v>64.67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65.29</c:v>
+                  <c:v>65.290000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>63.98</c:v>
@@ -371,11 +392,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2146144072"/>
-        <c:axId val="2146147480"/>
+        <c:axId val="-447955760"/>
+        <c:axId val="-447965552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2146144072"/>
+        <c:axId val="-447955760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,7 +412,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Language</a:t>
                 </a:r>
               </a:p>
@@ -400,10 +421,21 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146147480"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-447965552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -411,7 +443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146147480"/>
+        <c:axId val="-447965552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +460,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1800"/>
                   <a:t>Phone Error Rate</a:t>
                 </a:r>
               </a:p>
@@ -441,24 +473,29 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146144072"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-447955760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -822,38 +859,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16">
+    <row r="2" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>100.51</v>
@@ -861,8 +898,8 @@
       <c r="C2">
         <v>71.55</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="E2">
         <v>88.05</v>
@@ -874,9 +911,9 @@
         <v>48.08</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>106.45</v>
@@ -884,8 +921,8 @@
       <c r="C3">
         <v>96.21</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E3">
         <v>87.4</v>
@@ -897,9 +934,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>109.43</v>
@@ -907,8 +944,8 @@
       <c r="C4">
         <v>98.47</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E4">
         <v>88.86</v>
@@ -920,9 +957,9 @@
         <v>70.88</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>130.6</v>
@@ -930,8 +967,8 @@
       <c r="C5">
         <v>118.4</v>
       </c>
-      <c r="D5" t="s">
-        <v>3</v>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E5">
         <v>97.95</v>
@@ -943,9 +980,9 @@
         <v>64.67</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>91.85</v>
@@ -953,8 +990,8 @@
       <c r="C6">
         <v>78.31</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E6">
         <v>79.040000000000006</v>
@@ -966,9 +1003,9 @@
         <v>65.290000000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16">
+    <row r="7" spans="1:7" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>105.22</v>
@@ -976,8 +1013,8 @@
       <c r="C7">
         <v>97.18</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E7">
         <v>92.87</v>
@@ -991,8 +1028,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>